<commit_message>
Add back `Direct` and `HandFetched` fields
</commit_message>
<xml_diff>
--- a/template_v5.xlsx
+++ b/template_v5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardonpa/Library/CloudStorage/GoogleDrive-ricardo.npa@gmail.com/Shared drives/Development/Codes/ULTERA-contribute/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300F048D-A6DF-E94F-8035-C53B53079BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D95997A-3E1E-EE44-90BD-ACA574A8CF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>Ricardo Amaral</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{E96F1E22-8AF7-4549-A92A-92771E740A5E}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{E96F1E22-8AF7-4549-A92A-92771E740A5E}">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{2CEE6EAD-75A6-4549-883B-5E3A878E9A27}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{2CEE6EAD-75A6-4549-883B-5E3A878E9A27}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{320C2CDD-4C89-DB4E-B51B-C13A5633508B}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{320C2CDD-4C89-DB4E-B51B-C13A5633508B}">
       <text>
         <r>
           <rPr>
@@ -138,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{65F80236-A91C-C84E-AD18-C26E4246405A}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{65F80236-A91C-C84E-AD18-C26E4246405A}">
       <text>
         <r>
           <rPr>
@@ -174,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{BFC972C1-803D-EB4E-A665-C384DB5745CE}">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{BFC972C1-803D-EB4E-A665-C384DB5745CE}">
       <text>
         <r>
           <rPr>
@@ -199,7 +199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{79005E84-B4DA-AA46-9FA6-772836CB5A09}">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{79005E84-B4DA-AA46-9FA6-772836CB5A09}">
       <text>
         <r>
           <rPr>
@@ -224,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{B37A206A-5A80-DD42-806C-FFEA2312C097}">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{B37A206A-5A80-DD42-806C-FFEA2312C097}">
       <text>
         <r>
           <rPr>
@@ -260,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{C55305BE-16A2-754E-B180-DAF86A1A9915}">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{C55305BE-16A2-754E-B180-DAF86A1A9915}">
       <text>
         <r>
           <rPr>
@@ -296,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{BB0F128B-4254-6E40-A21D-B2C877863059}">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{BB0F128B-4254-6E40-A21D-B2C877863059}">
       <text>
         <r>
           <rPr>
@@ -321,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{C151D1A1-5112-D442-B098-E11EAA8E62B8}">
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{C151D1A1-5112-D442-B098-E11EAA8E62B8}">
       <text>
         <r>
           <rPr>
@@ -357,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{F4344F73-F2C0-A74D-9DC8-B7077165E8AE}">
+    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{F4344F73-F2C0-A74D-9DC8-B7077165E8AE}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{195D38B1-D5BE-714E-8570-038A43D66A64}">
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{195D38B1-D5BE-714E-8570-038A43D66A64}">
       <text>
         <r>
           <rPr>
@@ -418,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{08F55547-0581-6146-90A8-19B7C86222D6}">
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{08F55547-0581-6146-90A8-19B7C86222D6}">
       <text>
         <r>
           <rPr>
@@ -454,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{659A5507-B405-C742-B535-01CDB614FC6B}">
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{659A5507-B405-C742-B535-01CDB614FC6B}">
       <text>
         <r>
           <rPr>
@@ -473,7 +473,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Name:</t>
   </si>
@@ -544,9 +544,6 @@
     <t>Optional Upload Comments</t>
   </si>
   <si>
-    <t>Optional Comment</t>
-  </si>
-  <si>
     <t>email@institutional.domain</t>
   </si>
   <si>
@@ -608,6 +605,15 @@
   </si>
   <si>
     <t>aging time 6 h</t>
+  </si>
+  <si>
+    <t>Direct:</t>
+  </si>
+  <si>
+    <t>HandFetched:</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1129,6 +1135,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1168,41 +1210,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1490,11 +1499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CF407"/>
+  <dimension ref="A1:CF409"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1524,24 +1533,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="44" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="58"/>
       <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
@@ -1552,23 +1561,21 @@
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
-        <v>25</v>
+      <c r="B2" s="63" t="s">
+        <v>24</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
       <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
@@ -1579,21 +1586,21 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>24</v>
+      <c r="B3" s="66" t="s">
+        <v>23</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
       <c r="P3"/>
       <c r="Q3"/>
       <c r="R3"/>
@@ -1601,315 +1608,333 @@
       <c r="T3"/>
     </row>
     <row r="4" spans="1:78" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
+      <c r="A4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
     </row>
-    <row r="5" spans="1:78" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:78" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="1:78" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+    </row>
+    <row r="7" spans="1:78" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="E7" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>35</v>
+      <c r="I7" s="40">
+        <v>298</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>37</v>
+      <c r="J7" s="41" t="s">
+        <v>17</v>
       </c>
-      <c r="E5" s="40" t="s">
-        <v>44</v>
+      <c r="K7" s="41" t="s">
+        <v>41</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="L7" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="40">
-        <v>298</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" s="40" t="s">
+      <c r="N7" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="57" t="s">
-        <v>34</v>
+      <c r="P7" s="44" t="s">
+        <v>33</v>
       </c>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="40"/>
-      <c r="AA5" s="40"/>
-      <c r="AB5" s="40"/>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="40"/>
-      <c r="AE5" s="40"/>
-      <c r="AF5" s="40"/>
-      <c r="AG5" s="40"/>
-      <c r="AH5" s="40"/>
-      <c r="AI5" s="40"/>
-      <c r="AJ5" s="40"/>
-      <c r="AK5" s="40"/>
-      <c r="AL5" s="40"/>
-      <c r="AM5" s="40"/>
-      <c r="AN5" s="40"/>
-      <c r="AO5" s="40"/>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
-      <c r="AS5" s="40"/>
-      <c r="AT5" s="40"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="40"/>
-      <c r="AW5" s="40"/>
-      <c r="AX5" s="40"/>
-      <c r="AY5" s="40"/>
-      <c r="AZ5" s="40"/>
-      <c r="BA5" s="40"/>
-      <c r="BB5" s="40"/>
-      <c r="BC5" s="40"/>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="40"/>
-      <c r="BF5" s="40"/>
-      <c r="BG5" s="40"/>
-      <c r="BH5" s="40"/>
-      <c r="BI5" s="40"/>
-      <c r="BJ5" s="40"/>
-      <c r="BK5" s="40"/>
-      <c r="BL5" s="40"/>
-      <c r="BM5" s="40"/>
-      <c r="BN5" s="40"/>
-      <c r="BO5" s="40"/>
-      <c r="BP5" s="40"/>
-      <c r="BQ5" s="40"/>
-      <c r="BR5" s="40"/>
-      <c r="BS5" s="40"/>
-      <c r="BT5" s="40"/>
-      <c r="BU5" s="40"/>
-      <c r="BV5" s="40"/>
-      <c r="BW5" s="40"/>
-      <c r="BX5" s="40"/>
-      <c r="BY5" s="40"/>
-      <c r="BZ5" s="40"/>
-    </row>
-    <row r="6" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="44"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="40"/>
+      <c r="Z7" s="40"/>
+      <c r="AA7" s="40"/>
+      <c r="AB7" s="40"/>
+      <c r="AC7" s="40"/>
+      <c r="AD7" s="40"/>
+      <c r="AE7" s="40"/>
+      <c r="AF7" s="40"/>
+      <c r="AG7" s="40"/>
+      <c r="AH7" s="40"/>
+      <c r="AI7" s="40"/>
+      <c r="AJ7" s="40"/>
+      <c r="AK7" s="40"/>
+      <c r="AL7" s="40"/>
+      <c r="AM7" s="40"/>
+      <c r="AN7" s="40"/>
+      <c r="AO7" s="40"/>
+      <c r="AP7" s="40"/>
+      <c r="AQ7" s="40"/>
+      <c r="AR7" s="40"/>
+      <c r="AS7" s="40"/>
+      <c r="AT7" s="40"/>
+      <c r="AU7" s="40"/>
+      <c r="AV7" s="40"/>
+      <c r="AW7" s="40"/>
+      <c r="AX7" s="40"/>
+      <c r="AY7" s="40"/>
+      <c r="AZ7" s="40"/>
+      <c r="BA7" s="40"/>
+      <c r="BB7" s="40"/>
+      <c r="BC7" s="40"/>
+      <c r="BD7" s="40"/>
+      <c r="BE7" s="40"/>
+      <c r="BF7" s="40"/>
+      <c r="BG7" s="40"/>
+      <c r="BH7" s="40"/>
+      <c r="BI7" s="40"/>
+      <c r="BJ7" s="40"/>
+      <c r="BK7" s="40"/>
+      <c r="BL7" s="40"/>
+      <c r="BM7" s="40"/>
+      <c r="BN7" s="40"/>
+      <c r="BO7" s="40"/>
+      <c r="BP7" s="40"/>
+      <c r="BQ7" s="40"/>
+      <c r="BR7" s="40"/>
+      <c r="BS7" s="40"/>
+      <c r="BT7" s="40"/>
+      <c r="BU7" s="40"/>
+      <c r="BV7" s="40"/>
+      <c r="BW7" s="40"/>
+      <c r="BX7" s="40"/>
+      <c r="BY7" s="40"/>
+      <c r="BZ7" s="40"/>
+    </row>
+    <row r="8" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="55"/>
+      <c r="P8" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="61" t="s">
-        <v>3</v>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="47"/>
+    </row>
+    <row r="9" spans="1:78" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>25</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64" t="s">
-        <v>8</v>
+      <c r="B9" s="11" t="s">
+        <v>4</v>
       </c>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="67" t="s">
-        <v>11</v>
+      <c r="C9" s="12" t="s">
+        <v>5</v>
       </c>
-      <c r="N6" s="68"/>
-      <c r="P6" s="58" t="s">
+      <c r="D9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="60"/>
-    </row>
-    <row r="7" spans="1:78" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="27" t="s">
+      <c r="Q9" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="28" t="s">
+      <c r="R9" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="R7" s="28" t="s">
+      <c r="S9" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="28" t="s">
+      <c r="T9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T7" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38"/>
-      <c r="AC7" s="38"/>
-      <c r="AD7" s="38"/>
-      <c r="AE7" s="38"/>
-      <c r="AF7" s="38"/>
-      <c r="AG7" s="38"/>
-      <c r="AH7" s="38"/>
-      <c r="AI7" s="38"/>
-      <c r="AJ7" s="38"/>
-      <c r="AK7" s="38"/>
-      <c r="AL7" s="38"/>
-      <c r="AM7" s="38"/>
-      <c r="AN7" s="38"/>
-      <c r="AO7" s="38"/>
-      <c r="AP7" s="38"/>
-      <c r="AQ7" s="38"/>
-      <c r="AR7" s="38"/>
-      <c r="AS7" s="38"/>
-      <c r="AT7" s="38"/>
-      <c r="AU7" s="38"/>
-      <c r="AV7" s="38"/>
-      <c r="AW7" s="38"/>
-      <c r="AX7" s="38"/>
-      <c r="AY7" s="38"/>
-      <c r="AZ7" s="38"/>
-      <c r="BA7" s="38"/>
-      <c r="BB7" s="38"/>
-      <c r="BC7" s="38"/>
-      <c r="BD7" s="38"/>
-      <c r="BE7" s="38"/>
-      <c r="BF7" s="38"/>
-      <c r="BG7" s="38"/>
-      <c r="BH7" s="38"/>
-      <c r="BI7" s="38"/>
-      <c r="BJ7" s="38"/>
-      <c r="BK7" s="38"/>
-      <c r="BL7" s="38"/>
-      <c r="BM7" s="38"/>
-      <c r="BN7" s="38"/>
-      <c r="BO7" s="38"/>
-      <c r="BP7" s="38"/>
-      <c r="BQ7" s="38"/>
-      <c r="BR7" s="38"/>
-      <c r="BS7" s="38"/>
-      <c r="BT7" s="38"/>
-      <c r="BU7" s="38"/>
-      <c r="BV7" s="38"/>
-      <c r="BW7" s="38"/>
-      <c r="BX7" s="38"/>
-      <c r="BY7" s="38"/>
-      <c r="BZ7" s="38"/>
-    </row>
-    <row r="9" spans="1:78" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K9" s="2"/>
-    </row>
-    <row r="20" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="7"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="38"/>
+      <c r="AJ9" s="38"/>
+      <c r="AK9" s="38"/>
+      <c r="AL9" s="38"/>
+      <c r="AM9" s="38"/>
+      <c r="AN9" s="38"/>
+      <c r="AO9" s="38"/>
+      <c r="AP9" s="38"/>
+      <c r="AQ9" s="38"/>
+      <c r="AR9" s="38"/>
+      <c r="AS9" s="38"/>
+      <c r="AT9" s="38"/>
+      <c r="AU9" s="38"/>
+      <c r="AV9" s="38"/>
+      <c r="AW9" s="38"/>
+      <c r="AX9" s="38"/>
+      <c r="AY9" s="38"/>
+      <c r="AZ9" s="38"/>
+      <c r="BA9" s="38"/>
+      <c r="BB9" s="38"/>
+      <c r="BC9" s="38"/>
+      <c r="BD9" s="38"/>
+      <c r="BE9" s="38"/>
+      <c r="BF9" s="38"/>
+      <c r="BG9" s="38"/>
+      <c r="BH9" s="38"/>
+      <c r="BI9" s="38"/>
+      <c r="BJ9" s="38"/>
+      <c r="BK9" s="38"/>
+      <c r="BL9" s="38"/>
+      <c r="BM9" s="38"/>
+      <c r="BN9" s="38"/>
+      <c r="BO9" s="38"/>
+      <c r="BP9" s="38"/>
+      <c r="BQ9" s="38"/>
+      <c r="BR9" s="38"/>
+      <c r="BS9" s="38"/>
+      <c r="BT9" s="38"/>
+      <c r="BU9" s="38"/>
+      <c r="BV9" s="38"/>
+      <c r="BW9" s="38"/>
+      <c r="BX9" s="38"/>
+      <c r="BY9" s="38"/>
+      <c r="BZ9" s="38"/>
+    </row>
+    <row r="11" spans="1:78" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="2"/>
     </row>
     <row r="22" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
@@ -1928,24 +1953,20 @@
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="16"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="16"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="36"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="7"/>
     </row>
     <row r="24" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
@@ -1964,20 +1985,24 @@
       <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="7"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="16"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="16"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="36"/>
     </row>
     <row r="26" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
@@ -2001,7 +2026,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="6"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
@@ -5340,6 +5365,14 @@
       <c r="N235" s="7"/>
     </row>
     <row r="236" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="17"/>
+      <c r="B236" s="6"/>
+      <c r="C236" s="2"/>
+      <c r="D236" s="2"/>
+      <c r="E236" s="7"/>
+      <c r="F236" s="6"/>
+      <c r="G236" s="2"/>
+      <c r="H236" s="2"/>
       <c r="I236" s="3"/>
       <c r="J236" s="4"/>
       <c r="K236" s="4"/>
@@ -5348,6 +5381,14 @@
       <c r="N236" s="7"/>
     </row>
     <row r="237" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="17"/>
+      <c r="B237" s="6"/>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
+      <c r="E237" s="7"/>
+      <c r="F237" s="6"/>
+      <c r="G237" s="2"/>
+      <c r="H237" s="2"/>
       <c r="I237" s="3"/>
       <c r="J237" s="4"/>
       <c r="K237" s="4"/>
@@ -6715,59 +6756,80 @@
       <c r="M407" s="6"/>
       <c r="N407" s="7"/>
     </row>
+    <row r="408" spans="9:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I408" s="3"/>
+      <c r="J408" s="4"/>
+      <c r="K408" s="4"/>
+      <c r="L408" s="7"/>
+      <c r="M408" s="6"/>
+      <c r="N408" s="7"/>
+    </row>
+    <row r="409" spans="9:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I409" s="3"/>
+      <c r="J409" s="4"/>
+      <c r="K409" s="4"/>
+      <c r="L409" s="7"/>
+      <c r="M409" s="6"/>
+      <c r="N409" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="P6:T6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:L6"/>
-    <mergeCell ref="M6:N6"/>
+  <mergeCells count="12">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F2:N5"/>
     <mergeCell ref="F1:N1"/>
-    <mergeCell ref="F2:N3"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="P7:T7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{A96D4568-3644-C442-861B-6177D116491B}">
-      <formula1>"BCC, FCC, BCT, HCP, B2, L12, L10, D03, MC, MB2, laves, sigma, gamma, martensite, amorphous, Ti2Ni, Al3Zr5, BCC+laves, BCC+BCC, other.."</formula1>
+  <dataValidations count="14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{A96D4568-3644-C442-861B-6177D116491B}">
+      <formula1>"BCC+laves, BCC+BCC, BCC, FCC, BCT, HCP, B2, L12, L10, D03, MC, MB2, laves, sigma, gamma, martensite, amorphous, Ti2Ni, Al3Zr5, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{F4278397-5895-994C-AA24-F61B63DEED5C}">
-      <formula1>"AC, VAM, AAM, VIM, VC, DC, PC, IC, RS, MS, MA, BM, SPS, HIP, AM, SLM, SLS, DED, A, H, RX, N, SR, AQ, WQ, OQ, HW, CW, SPD, HE, CE, HR, CR, AT, CT, ST, C, N, PS, SC, SD, TE, CVD, CP, PC, BM+HIP+A, .."</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7" xr:uid="{F4278397-5895-994C-AA24-F61B63DEED5C}">
+      <formula1>"A+WQ, BM+HIP+A, AC, VAM, AAM, VIM, VC, DC, PC, IC, RS, MS, MA, BM, SPS, HIP, AM, SLM, SLS, DED, A, H, RX, N, SR, AQ, WQ, OQ, HW, CW, SPD, HE, CE, HR, CR, AT, CT, ST, C, N, PS, SC, SD, TE, CVD, CP, PC, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{5311D079-2B17-9041-A27B-C52D45844D97}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{5311D079-2B17-9041-A27B-C52D45844D97}">
       <formula1>"Cr0.1 Fe0.1 Ni0.8, Nb9 Hf Co3, Cr Fe Mg Ni"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5" xr:uid="{1F0F94DB-36A3-FA4A-8916-D53CE4398E19}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7" xr:uid="{1F0F94DB-36A3-FA4A-8916-D53CE4398E19}">
       <formula1>"EXP, EMP, ML, DFT, CAL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{C5340290-0E2D-0D40-8C05-0DB4A4520240}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7" xr:uid="{C5340290-0E2D-0D40-8C05-0DB4A4520240}">
       <formula1>"density, melting temperature, tensile yield strength, ultimate tensile strength, fracture tensile strength, tensile ductility, youngs modulus, bulk modulus, poissons ratio, hardness, nanohardness, fracture toughness, thermal conductivity, creep rate, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5" xr:uid="{15C1A934-8D9B-B84B-9CB9-FC3A0F25228A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7" xr:uid="{15C1A934-8D9B-B84B-9CB9-FC3A0F25228A}">
       <formula1>"strain rate 1e-3 s-1, max stress 120e6 Pa, load 100 g, other.."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5" xr:uid="{7530AD0D-F2E0-A141-897F-F3D8E476ECE8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7" xr:uid="{7530AD0D-F2E0-A141-897F-F3D8E476ECE8}">
       <formula1>"10.1557/jmr.2018.153, Senkov_2018_DevelopmentAndExploration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5" xr:uid="{326A014A-ED27-B54A-82FC-B96E9CA4C033}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7" xr:uid="{326A014A-ED27-B54A-82FC-B96E9CA4C033}">
       <formula1>"F7, T2, P3, SF2, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5" xr:uid="{4A229DBE-A808-C842-8CB6-48556B8DE873}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7" xr:uid="{4A229DBE-A808-C842-8CB6-48556B8DE873}">
       <formula1>"Pa, m3, kg, s-1, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5" xr:uid="{9F29C709-5D87-1843-8091-46C3173B9CEA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7" xr:uid="{9F29C709-5D87-1843-8091-46C3173B9CEA}">
       <formula1>"1e6, 1000000, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5" xr:uid="{B3B3F5ED-1A0D-4D48-AC8D-3005D0CD4979}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7" xr:uid="{B3B3F5ED-1A0D-4D48-AC8D-3005D0CD4979}">
       <formula1>"5e6, 5000000, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5" xr:uid="{58429272-7ACB-4B46-A25F-991C256FF94A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7" xr:uid="{58429272-7ACB-4B46-A25F-991C256FF94A}">
       <formula1>"298, 1000, .."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5" xr:uid="{AF7275B5-D11D-BB48-8DF5-349BB40D1805}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{AF7275B5-D11D-BB48-8DF5-349BB40D1805}">
       <formula1>"aging time 6 h, grain size 1 micron, thickness 2 mm, .."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:E5" xr:uid="{A5A9FEF4-8BD7-4040-8635-44DEF8431CDE}">
+      <formula1>"T, F"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -6776,7 +6838,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="J5:K5" numberStoredAsText="1"/>
+    <ignoredError sqref="J7:K7" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>